<commit_message>
Implementación CU-30 y 31
Se implementaron los CU de Editar cliente y consultar información del cliente, además de realizar los respectivos diagramas de cada uno
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 6/Plantilla Lista de Tareas de la Entrega 6.xlsx
+++ b/Plantillas/Entrega 6/Plantilla Lista de Tareas de la Entrega 6.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001686D5-3502-4AC6-8C32-9C9FA9F8A53C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A21DD2D-D2F2-45D9-84E6-B191DCEB5023}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
   <si>
     <t>Columna</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>El director podrá modificar el horario existente</t>
+  </si>
+  <si>
+    <t>Hecho</t>
   </si>
 </sst>
 </file>
@@ -886,10 +889,10 @@
   <dimension ref="B1:BB39"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="S8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1539,7 @@
         <v>41</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="G10" s="24">
         <v>2</v>
@@ -1650,7 +1653,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="G11" s="24">
         <v>2</v>
@@ -1764,7 +1767,7 @@
         <v>41</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="G12" s="24">
         <v>2</v>
@@ -1799,72 +1802,74 @@
         <v>2</v>
       </c>
       <c r="V12" s="20"/>
-      <c r="W12" s="20"/>
+      <c r="W12" s="20">
+        <v>0.5</v>
+      </c>
       <c r="X12" s="20">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="Y12" s="20"/>
       <c r="Z12" s="20"/>
       <c r="AA12" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB12" s="20"/>
       <c r="AC12" s="20"/>
       <c r="AD12" s="20">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AE12" s="20"/>
       <c r="AF12" s="20"/>
       <c r="AG12" s="20">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AH12" s="20"/>
       <c r="AI12" s="20"/>
       <c r="AJ12" s="20">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AK12" s="20"/>
       <c r="AL12" s="20"/>
       <c r="AM12" s="20">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AN12" s="20"/>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AQ12" s="20"/>
       <c r="AR12" s="20"/>
       <c r="AS12" s="20">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AT12" s="20"/>
       <c r="AU12" s="20"/>
       <c r="AV12" s="20">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AW12" s="20"/>
       <c r="AX12" s="20"/>
       <c r="AY12" s="20">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AZ12" s="33">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA12" s="33">
         <f>G12-AZ12</f>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BB12" s="2"/>
     </row>
@@ -1878,7 +1883,7 @@
         <v>41</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="G13" s="24">
         <v>2</v>
@@ -1931,54 +1936,56 @@
         <v>2</v>
       </c>
       <c r="AE13" s="20"/>
-      <c r="AF13" s="20"/>
+      <c r="AF13" s="20">
+        <v>2</v>
+      </c>
       <c r="AG13" s="20">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH13" s="20"/>
       <c r="AI13" s="20"/>
       <c r="AJ13" s="20">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK13" s="20"/>
       <c r="AL13" s="20"/>
       <c r="AM13" s="20">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ13" s="20"/>
       <c r="AR13" s="20"/>
       <c r="AS13" s="20">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT13" s="20"/>
       <c r="AU13" s="20"/>
       <c r="AV13" s="20">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW13" s="20"/>
       <c r="AX13" s="20"/>
       <c r="AY13" s="20">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ13" s="33">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA13" s="33">
         <f t="shared" ref="BA13:BA20" si="19">G13-AZ13</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BB13" s="2"/>
     </row>
@@ -2165,7 +2172,7 @@
         <v>41</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G16" s="24">
         <v>2</v>
@@ -2206,66 +2213,68 @@
         <v>2</v>
       </c>
       <c r="Y16" s="20"/>
-      <c r="Z16" s="20"/>
+      <c r="Z16" s="20">
+        <v>1</v>
+      </c>
       <c r="AA16" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB16" s="20"/>
       <c r="AC16" s="20"/>
       <c r="AD16" s="20">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE16" s="20"/>
       <c r="AF16" s="20"/>
       <c r="AG16" s="20">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH16" s="20"/>
       <c r="AI16" s="20"/>
       <c r="AJ16" s="20">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK16" s="20"/>
       <c r="AL16" s="20"/>
       <c r="AM16" s="20">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN16" s="20"/>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ16" s="20"/>
       <c r="AR16" s="20"/>
       <c r="AS16" s="20">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT16" s="20"/>
       <c r="AU16" s="20"/>
       <c r="AV16" s="20">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW16" s="20"/>
       <c r="AX16" s="20"/>
       <c r="AY16" s="20">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ16" s="33">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA16" s="33">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB16" s="2"/>
     </row>
@@ -2279,7 +2288,7 @@
         <v>41</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G17" s="24">
         <v>2</v>
@@ -2320,66 +2329,68 @@
         <v>2</v>
       </c>
       <c r="Y17" s="20"/>
-      <c r="Z17" s="20"/>
+      <c r="Z17" s="20">
+        <v>1</v>
+      </c>
       <c r="AA17" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB17" s="20"/>
       <c r="AC17" s="20"/>
       <c r="AD17" s="20">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE17" s="20"/>
       <c r="AF17" s="20"/>
       <c r="AG17" s="20">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH17" s="20"/>
       <c r="AI17" s="20"/>
       <c r="AJ17" s="20">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK17" s="20"/>
       <c r="AL17" s="20"/>
       <c r="AM17" s="20">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN17" s="20"/>
       <c r="AO17" s="20"/>
       <c r="AP17" s="20">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ17" s="20"/>
       <c r="AR17" s="20"/>
       <c r="AS17" s="20">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT17" s="20"/>
       <c r="AU17" s="20"/>
       <c r="AV17" s="20">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW17" s="20"/>
       <c r="AX17" s="20"/>
       <c r="AY17" s="20">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ17" s="33">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA17" s="33">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB17" s="2"/>
     </row>
@@ -2393,7 +2404,7 @@
         <v>41</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G18" s="24">
         <v>2</v>
@@ -2428,72 +2439,74 @@
         <v>2</v>
       </c>
       <c r="V18" s="20"/>
-      <c r="W18" s="20"/>
+      <c r="W18" s="20">
+        <v>0.5</v>
+      </c>
       <c r="X18" s="20">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="Y18" s="20"/>
       <c r="Z18" s="20"/>
       <c r="AA18" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB18" s="20"/>
       <c r="AC18" s="20"/>
       <c r="AD18" s="20">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AE18" s="20"/>
       <c r="AF18" s="20"/>
       <c r="AG18" s="20">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AH18" s="20"/>
       <c r="AI18" s="20"/>
       <c r="AJ18" s="20">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AK18" s="20"/>
       <c r="AL18" s="20"/>
       <c r="AM18" s="20">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AN18" s="20"/>
       <c r="AO18" s="20"/>
       <c r="AP18" s="20">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AQ18" s="20"/>
       <c r="AR18" s="20"/>
       <c r="AS18" s="20">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AT18" s="20"/>
       <c r="AU18" s="20"/>
       <c r="AV18" s="20">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AW18" s="20"/>
       <c r="AX18" s="20"/>
       <c r="AY18" s="20">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AZ18" s="33">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA18" s="33">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="BB18" s="2"/>
     </row>
@@ -2507,7 +2520,7 @@
         <v>41</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G19" s="24">
         <v>3</v>
@@ -2554,60 +2567,64 @@
         <v>3</v>
       </c>
       <c r="AB19" s="20"/>
-      <c r="AC19" s="20"/>
+      <c r="AC19" s="20">
+        <v>1</v>
+      </c>
       <c r="AD19" s="20">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE19" s="20"/>
-      <c r="AF19" s="20"/>
+      <c r="AF19" s="20">
+        <v>1</v>
+      </c>
       <c r="AG19" s="20">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AH19" s="20"/>
       <c r="AI19" s="20"/>
       <c r="AJ19" s="20">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK19" s="20"/>
       <c r="AL19" s="20"/>
       <c r="AM19" s="20">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AN19" s="20"/>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AQ19" s="20"/>
       <c r="AR19" s="20"/>
       <c r="AS19" s="20">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AT19" s="20"/>
       <c r="AU19" s="20"/>
       <c r="AV19" s="20">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AW19" s="20"/>
       <c r="AX19" s="20"/>
       <c r="AY19" s="20">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AZ19" s="33">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA19" s="33">
         <f t="shared" si="19"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BB19" s="2"/>
     </row>
@@ -4557,11 +4574,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -4573,6 +4585,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Pruebas untarias y registro de tiempos
Se crearon la pruebas unitaria de crear renta, se registraron los tiempos de la iteración, así como los de los CU y se actualizó el plan de pruebas
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 6/Plantilla Lista de Tareas de la Entrega 6.xlsx
+++ b/Plantillas/Entrega 6/Plantilla Lista de Tareas de la Entrega 6.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B396AA-EA42-4F0E-94CB-206D7A867BF1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C955CD4-74F6-4F80-9621-E83B0593D548}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -936,10 +936,10 @@
   <dimension ref="B1:BB64"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AK6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AQ53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="Y62" sqref="Y62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6013,66 +6013,74 @@
         <v>15</v>
       </c>
       <c r="Y52" s="36"/>
-      <c r="Z52" s="36"/>
+      <c r="Z52" s="36">
+        <v>3</v>
+      </c>
       <c r="AA52" s="36">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AB52" s="36"/>
-      <c r="AC52" s="36"/>
+      <c r="AC52" s="36">
+        <v>2</v>
+      </c>
       <c r="AD52" s="36">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AE52" s="36"/>
-      <c r="AF52" s="36"/>
+      <c r="AF52" s="36">
+        <v>5</v>
+      </c>
       <c r="AG52" s="36">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="AH52" s="36"/>
-      <c r="AI52" s="36"/>
+      <c r="AI52" s="36">
+        <v>3</v>
+      </c>
       <c r="AJ52" s="36">
         <f t="shared" si="9"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AK52" s="36"/>
       <c r="AL52" s="36"/>
       <c r="AM52" s="36">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AN52" s="36"/>
       <c r="AO52" s="36"/>
       <c r="AP52" s="36">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AQ52" s="36"/>
       <c r="AR52" s="36"/>
       <c r="AS52" s="36">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AT52" s="36"/>
       <c r="AU52" s="36"/>
       <c r="AV52" s="36">
         <f t="shared" si="13"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AW52" s="36"/>
       <c r="AX52" s="36"/>
       <c r="AY52" s="36">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AZ52" s="32">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="BA52" s="32">
         <f>G52-AZ52</f>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="BB52" s="2"/>
     </row>
@@ -6163,30 +6171,32 @@
         <v>4</v>
       </c>
       <c r="AQ53" s="36"/>
-      <c r="AR53" s="36"/>
+      <c r="AR53" s="36">
+        <v>1</v>
+      </c>
       <c r="AS53" s="36">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AT53" s="36"/>
       <c r="AU53" s="36"/>
       <c r="AV53" s="36">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AW53" s="36"/>
       <c r="AX53" s="36"/>
       <c r="AY53" s="36">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AZ53" s="32">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA53" s="32">
         <f>G53-AZ53</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BB53" s="2"/>
     </row>
@@ -6282,88 +6292,90 @@
         <v>2</v>
       </c>
       <c r="P55" s="36"/>
-      <c r="Q55" s="36"/>
+      <c r="Q55" s="36">
+        <v>1.5</v>
+      </c>
       <c r="R55" s="36">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="S55" s="36"/>
       <c r="T55" s="36"/>
       <c r="U55" s="36">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="V55" s="36"/>
       <c r="W55" s="36"/>
       <c r="X55" s="36">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="Y55" s="36"/>
       <c r="Z55" s="36"/>
       <c r="AA55" s="36">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AB55" s="36"/>
       <c r="AC55" s="36"/>
       <c r="AD55" s="36">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AE55" s="36"/>
       <c r="AF55" s="36"/>
       <c r="AG55" s="36">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AH55" s="36"/>
       <c r="AI55" s="36"/>
       <c r="AJ55" s="36">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AK55" s="36"/>
       <c r="AL55" s="36"/>
       <c r="AM55" s="36">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AN55" s="36"/>
       <c r="AO55" s="36"/>
       <c r="AP55" s="36">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AQ55" s="36"/>
       <c r="AR55" s="36"/>
       <c r="AS55" s="36">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AT55" s="36"/>
       <c r="AU55" s="36"/>
       <c r="AV55" s="36">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AW55" s="36"/>
       <c r="AX55" s="36"/>
       <c r="AY55" s="36">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AZ55" s="32">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="BA55" s="32">
         <f>G55-AZ55</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="BB55" s="2"/>
     </row>
-    <row r="56" spans="2:54" s="38" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:54" s="38" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="39" t="s">
         <v>54</v>
       </c>
@@ -6443,96 +6455,98 @@
         <v>2</v>
       </c>
       <c r="J57" s="36"/>
-      <c r="K57" s="36"/>
+      <c r="K57" s="36">
+        <v>1</v>
+      </c>
       <c r="L57" s="36">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M57" s="36"/>
       <c r="N57" s="36"/>
       <c r="O57" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P57" s="36"/>
       <c r="Q57" s="36"/>
       <c r="R57" s="36">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S57" s="36"/>
       <c r="T57" s="36"/>
       <c r="U57" s="36">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V57" s="36"/>
       <c r="W57" s="36"/>
       <c r="X57" s="36">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y57" s="36"/>
       <c r="Z57" s="36"/>
       <c r="AA57" s="36">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB57" s="36"/>
       <c r="AC57" s="36"/>
       <c r="AD57" s="36">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE57" s="36"/>
       <c r="AF57" s="36"/>
       <c r="AG57" s="36">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH57" s="36"/>
       <c r="AI57" s="36"/>
       <c r="AJ57" s="36">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK57" s="36"/>
       <c r="AL57" s="36"/>
       <c r="AM57" s="36">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN57" s="36"/>
       <c r="AO57" s="36"/>
       <c r="AP57" s="36">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ57" s="36"/>
       <c r="AR57" s="36"/>
       <c r="AS57" s="36">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT57" s="36"/>
       <c r="AU57" s="36"/>
       <c r="AV57" s="36">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW57" s="36"/>
       <c r="AX57" s="36"/>
       <c r="AY57" s="36">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ57" s="32">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA57" s="32">
         <f t="shared" ref="BA57:BA63" si="112">G57-AZ57</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB57" s="2"/>
     </row>
@@ -6557,96 +6571,98 @@
         <v>2</v>
       </c>
       <c r="J58" s="36"/>
-      <c r="K58" s="36"/>
+      <c r="K58" s="36">
+        <v>1</v>
+      </c>
       <c r="L58" s="36">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M58" s="36"/>
       <c r="N58" s="36"/>
       <c r="O58" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P58" s="36"/>
       <c r="Q58" s="36"/>
       <c r="R58" s="36">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S58" s="36"/>
       <c r="T58" s="36"/>
       <c r="U58" s="36">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V58" s="36"/>
       <c r="W58" s="36"/>
       <c r="X58" s="36">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y58" s="36"/>
       <c r="Z58" s="36"/>
       <c r="AA58" s="36">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB58" s="36"/>
       <c r="AC58" s="36"/>
       <c r="AD58" s="36">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE58" s="36"/>
       <c r="AF58" s="36"/>
       <c r="AG58" s="36">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH58" s="36"/>
       <c r="AI58" s="36"/>
       <c r="AJ58" s="36">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK58" s="36"/>
       <c r="AL58" s="36"/>
       <c r="AM58" s="36">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN58" s="36"/>
       <c r="AO58" s="36"/>
       <c r="AP58" s="36">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ58" s="36"/>
       <c r="AR58" s="36"/>
       <c r="AS58" s="36">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT58" s="36"/>
       <c r="AU58" s="36"/>
       <c r="AV58" s="36">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW58" s="36"/>
       <c r="AX58" s="36"/>
       <c r="AY58" s="36">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ58" s="32">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA58" s="32">
         <f t="shared" si="112"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB58" s="2"/>
     </row>
@@ -6736,90 +6752,92 @@
         <v>2</v>
       </c>
       <c r="M60" s="36"/>
-      <c r="N60" s="36"/>
+      <c r="N60" s="36">
+        <v>1</v>
+      </c>
       <c r="O60" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P60" s="36"/>
       <c r="Q60" s="36"/>
       <c r="R60" s="36">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S60" s="36"/>
       <c r="T60" s="36"/>
       <c r="U60" s="36">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V60" s="36"/>
       <c r="W60" s="36"/>
       <c r="X60" s="36">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y60" s="36"/>
       <c r="Z60" s="36"/>
       <c r="AA60" s="36">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB60" s="36"/>
       <c r="AC60" s="36"/>
       <c r="AD60" s="36">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE60" s="36"/>
       <c r="AF60" s="36"/>
       <c r="AG60" s="36">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH60" s="36"/>
       <c r="AI60" s="36"/>
       <c r="AJ60" s="36">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK60" s="36"/>
       <c r="AL60" s="36"/>
       <c r="AM60" s="36">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN60" s="36"/>
       <c r="AO60" s="36"/>
       <c r="AP60" s="36">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ60" s="36"/>
       <c r="AR60" s="36"/>
       <c r="AS60" s="36">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT60" s="36"/>
       <c r="AU60" s="36"/>
       <c r="AV60" s="36">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW60" s="36"/>
       <c r="AX60" s="36"/>
       <c r="AY60" s="36">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ60" s="32">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA60" s="32">
         <f t="shared" si="112"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB60" s="2"/>
     </row>
@@ -6850,90 +6868,92 @@
         <v>2</v>
       </c>
       <c r="M61" s="36"/>
-      <c r="N61" s="36"/>
+      <c r="N61" s="36">
+        <v>1</v>
+      </c>
       <c r="O61" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P61" s="36"/>
       <c r="Q61" s="36"/>
       <c r="R61" s="36">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S61" s="36"/>
       <c r="T61" s="36"/>
       <c r="U61" s="36">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V61" s="36"/>
       <c r="W61" s="36"/>
       <c r="X61" s="36">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y61" s="36"/>
       <c r="Z61" s="36"/>
       <c r="AA61" s="36">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB61" s="36"/>
       <c r="AC61" s="36"/>
       <c r="AD61" s="36">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE61" s="36"/>
       <c r="AF61" s="36"/>
       <c r="AG61" s="36">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH61" s="36"/>
       <c r="AI61" s="36"/>
       <c r="AJ61" s="36">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK61" s="36"/>
       <c r="AL61" s="36"/>
       <c r="AM61" s="36">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN61" s="36"/>
       <c r="AO61" s="36"/>
       <c r="AP61" s="36">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ61" s="36"/>
       <c r="AR61" s="36"/>
       <c r="AS61" s="36">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT61" s="36"/>
       <c r="AU61" s="36"/>
       <c r="AV61" s="36">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW61" s="36"/>
       <c r="AX61" s="36"/>
       <c r="AY61" s="36">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ61" s="32">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA61" s="32">
         <f t="shared" si="112"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB61" s="2"/>
     </row>
@@ -7163,11 +7183,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -7179,6 +7194,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>